<commit_message>
fixed text and excel date errors
</commit_message>
<xml_diff>
--- a/src/main/resources/carInfo.xlsx
+++ b/src/main/resources/carInfo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC105F98-ECC0-46B5-A2EA-C7570B553047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BEDF6E-FB86-4761-97C5-19DCB310BD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2664" yWindow="3552" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -130,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +474,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,6 +483,7 @@
     <col min="2" max="2" width="22.77734375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="26.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -520,8 +522,8 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2">
-        <v>2020</v>
+      <c r="E2" s="1">
+        <v>44135</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
@@ -543,8 +545,8 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
-        <v>2019</v>
+      <c r="E3" s="1">
+        <v>44135</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
@@ -566,8 +568,8 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4">
-        <v>2021</v>
+      <c r="E4" s="1">
+        <v>44135</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -589,8 +591,8 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5">
-        <v>2022</v>
+      <c r="E5" s="1">
+        <v>44135</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>

</xml_diff>